<commit_message>
addicion precio sin intereses
</commit_message>
<xml_diff>
--- a/Reporte/REPORTES DORA.xlsx
+++ b/Reporte/REPORTES DORA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GAIA\APIs Chats\WatsonComandato\apiWatson\Reporte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GAIA\chatbotComandato\apiWatson-master\Reporte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5BFFCA-7218-4CB3-BDA6-F5EC69E28050}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA43FD82-6C34-4643-A33C-AB1F2C0240D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intenciones Clientes" sheetId="1" r:id="rId1"/>
@@ -27,112 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="48">
-  <si>
-    <t>WHATSAPP</t>
-  </si>
-  <si>
-    <t>NOMBRES CLIENTE</t>
-  </si>
-  <si>
-    <t>TELEFONO CLIENTE</t>
-  </si>
-  <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>canalMensajeria</t>
-  </si>
-  <si>
-    <t>nombresCliente</t>
-  </si>
-  <si>
-    <t>telefonoCliente</t>
-  </si>
-  <si>
-    <t>numeroReferencia</t>
-  </si>
-  <si>
-    <t>fechaCreacion</t>
-  </si>
-  <si>
-    <t>fechaUltimaModificacion</t>
-  </si>
-  <si>
-    <t>fechaFinalizacion</t>
-  </si>
-  <si>
-    <t>cantidad</t>
-  </si>
-  <si>
-    <t>nombreProducto</t>
-  </si>
-  <si>
-    <t>idProductoBot</t>
-  </si>
-  <si>
-    <t>estadoDetalle</t>
-  </si>
-  <si>
-    <t>precioProducto</t>
-  </si>
-  <si>
-    <t>identificadorMetodoPago</t>
-  </si>
-  <si>
-    <t>metodoPago</t>
-  </si>
-  <si>
-    <t>creado</t>
-  </si>
-  <si>
-    <t>Dayana Helen</t>
-  </si>
-  <si>
-    <t>2020-08-23 10:47:44.960</t>
-  </si>
-  <si>
-    <t>2020-08-23 12:19:02.473</t>
-  </si>
-  <si>
-    <t>NULL</t>
-  </si>
-  <si>
-    <t>Oled LG OLED65C8 65" - Color Plateado</t>
-  </si>
-  <si>
-    <t>2507.56</t>
-  </si>
-  <si>
-    <t>Tarjeta de Crédito</t>
-  </si>
-  <si>
-    <t>Lavadora Automática -  Mabe - LMA70200WDAB1  | 20 Kg – Silver</t>
-  </si>
-  <si>
-    <t>487.64</t>
-  </si>
-  <si>
-    <t>finalizado</t>
-  </si>
-  <si>
-    <t>Héctor García</t>
-  </si>
-  <si>
-    <t>2020-08-23 13:05:17.153</t>
-  </si>
-  <si>
-    <t>2020-08-23 13:06:40.693</t>
-  </si>
-  <si>
-    <t>Tablet Lenovo TAB M10 - Pantalla 10.1" - Color Negro</t>
-  </si>
-  <si>
-    <t>500.04</t>
-  </si>
-  <si>
-    <t>Crédito Directo Comandato</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>INTENCIONES CLIENTES</t>
   </si>
@@ -142,78 +37,55 @@
   <si>
     <t>CANAL MENSAJERIA</t>
   </si>
-  <si>
-    <t>BRYAN AGRCIA</t>
-  </si>
-  <si>
-    <t>Marca</t>
-  </si>
-  <si>
-    <t>televisor</t>
-  </si>
-  <si>
-    <t>LG</t>
-  </si>
-  <si>
-    <t>Tipo Producto</t>
-  </si>
-  <si>
-    <t>Nombre Producto</t>
-  </si>
-  <si>
-    <t>Televisor</t>
-  </si>
-  <si>
-    <t>LED ZN56 + KIT LIMPIEZA</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>Dayana Bailon</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,12 +95,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0056B3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD8FF83"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,44 +135,42 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -316,8 +180,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0056B3"/>
       <color rgb="FFD8FF83"/>
-      <color rgb="FF0056B3"/>
     </mruColors>
   </colors>
   <extLst>
@@ -531,64 +395,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.75" style="10" customWidth="1"/>
-    <col min="2" max="2" width="29.125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="17.125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="16.375" customWidth="1"/>
-    <col min="5" max="27" width="9.375" customWidth="1"/>
+    <col min="1" max="1" width="22.75" style="13" customWidth="1"/>
+    <col min="2" max="2" width="29.125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="40.375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="16.375" style="11" customWidth="1"/>
+    <col min="5" max="27" width="9.375" style="11" customWidth="1"/>
+    <col min="28" max="16384" width="12.625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>36</v>
+      <c r="A1" s="3" t="s">
+        <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>37</v>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1592,1034 +1457,448 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73:D78"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.625" style="4"/>
-    <col min="2" max="2" width="18" style="4" customWidth="1"/>
-    <col min="3" max="3" width="32.375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="26.375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="41" style="4" customWidth="1"/>
-    <col min="6" max="24" width="9.375" style="4" customWidth="1"/>
-    <col min="25" max="16384" width="12.625" style="4"/>
+    <col min="1" max="1" width="24.75" style="6" customWidth="1"/>
+    <col min="2" max="2" width="37.5" style="8" customWidth="1"/>
+    <col min="3" max="3" width="32.375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="68.125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="41" style="8" customWidth="1"/>
+    <col min="6" max="24" width="9.375" style="8" customWidth="1"/>
+    <col min="25" max="16384" width="12.625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="5">
-        <v>980546307</v>
-      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="12"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="3">
-        <v>2</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="12"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="4">
-        <v>3</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
-        <v>2</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="5">
-        <v>98925516366</v>
-      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="12"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="3">
-        <v>2</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="12"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="4">
-        <v>3</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
-        <v>2</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="5">
-        <v>98925516366</v>
-      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="3">
-        <v>1</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="12"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="3">
-        <v>2</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="12"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="4">
-        <v>3</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A19" s="2"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
-        <v>2</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="5">
-        <v>98925516366</v>
-      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="3">
-        <v>1</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="12"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="3">
-        <v>2</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="12"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="4">
-        <v>3</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
-        <v>2</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="5">
-        <v>98925516366</v>
-      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="3">
-        <v>1</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="12"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="9"/>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="3">
-        <v>2</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="12"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="4">
-        <v>3</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="9"/>
     </row>
     <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A31" s="2"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4">
-        <v>2</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" s="5">
-        <v>98925516366</v>
-      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="10"/>
     </row>
     <row r="33" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="3">
-        <v>1</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="12"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="9"/>
     </row>
     <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="3">
-        <v>2</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E35" s="12"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="9"/>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="4">
-        <v>3</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="9"/>
     </row>
     <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A37" s="2"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4">
-        <v>2</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D38" s="5">
-        <v>98925516366</v>
-      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="10"/>
     </row>
     <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="A39" s="2"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
-        <v>1</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="12"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="9"/>
     </row>
     <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
-        <v>2</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D41" s="12"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="4">
-        <v>3</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A43" s="2"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="4">
-        <v>2</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D44" s="5">
-        <v>98925516366</v>
-      </c>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="A45" s="2"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3">
-        <v>1</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="12"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="9"/>
     </row>
     <row r="47" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="3">
-        <v>2</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D47" s="12"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="9"/>
     </row>
     <row r="48" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="4">
-        <v>3</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="B48" s="9"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="9"/>
     </row>
     <row r="49" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A49" s="2"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
     </row>
     <row r="50" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="4">
-        <v>2</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D50" s="5">
-        <v>98925516366</v>
-      </c>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="10"/>
     </row>
     <row r="51" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="A51" s="2"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3">
-        <v>1</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C52" s="13"/>
-      <c r="D52" s="12"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="9"/>
     </row>
     <row r="53" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="3">
-        <v>2</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D53" s="12"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="9"/>
     </row>
     <row r="54" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="4">
-        <v>3</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="B54" s="9"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="9"/>
     </row>
     <row r="55" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A55" s="2"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
     </row>
     <row r="56" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="4">
-        <v>2</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D56" s="5">
-        <v>98925516366</v>
-      </c>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="10"/>
     </row>
     <row r="57" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="A57" s="2"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
     </row>
     <row r="58" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="3">
-        <v>1</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C58" s="13"/>
-      <c r="D58" s="12"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="9"/>
     </row>
     <row r="59" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="3">
-        <v>2</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C59" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D59" s="12"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="9"/>
     </row>
     <row r="60" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="4">
-        <v>3</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="B60" s="9"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="9"/>
     </row>
     <row r="61" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A61" s="2"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
     </row>
     <row r="62" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="4">
-        <v>2</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D62" s="5">
-        <v>98925516366</v>
-      </c>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="10"/>
     </row>
     <row r="63" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B63" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D63" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="A63" s="2"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
     </row>
     <row r="64" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="3">
-        <v>1</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C64" s="13"/>
-      <c r="D64" s="12"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="9"/>
     </row>
     <row r="65" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="3">
-        <v>2</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C65" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D65" s="12"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="9"/>
     </row>
     <row r="66" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="4">
-        <v>3</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C66" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="B66" s="9"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="9"/>
     </row>
     <row r="67" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A67" s="2"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
     </row>
     <row r="68" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="4">
-        <v>2</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D68" s="5">
-        <v>98925516366</v>
-      </c>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="10"/>
     </row>
     <row r="69" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C69" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D69" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="A69" s="2"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
     </row>
     <row r="70" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="3">
-        <v>1</v>
-      </c>
-      <c r="B70" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C70" s="13"/>
-      <c r="D70" s="12"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="9"/>
     </row>
     <row r="71" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="3">
-        <v>2</v>
-      </c>
-      <c r="B71" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C71" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D71" s="12"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="9"/>
     </row>
     <row r="72" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="4">
-        <v>3</v>
-      </c>
-      <c r="B72" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C72" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D72" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="B72" s="9"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="9"/>
     </row>
     <row r="73" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A73" s="2"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
     </row>
     <row r="74" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="4">
-        <v>2</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C74" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D74" s="5">
-        <v>98925516366</v>
-      </c>
+      <c r="B74" s="9"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="10"/>
     </row>
     <row r="75" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D75" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="A75" s="2"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
     </row>
     <row r="76" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="3">
-        <v>1</v>
-      </c>
-      <c r="B76" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C76" s="13"/>
-      <c r="D76" s="12"/>
+      <c r="B76" s="9"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="9"/>
     </row>
     <row r="77" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="3">
-        <v>2</v>
-      </c>
-      <c r="B77" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C77" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D77" s="12"/>
+      <c r="B77" s="9"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="9"/>
     </row>
     <row r="78" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="4">
-        <v>3</v>
-      </c>
-      <c r="B78" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C78" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D78" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="B78" s="9"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="9"/>
     </row>
     <row r="79" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="80" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3546,261 +2825,80 @@
     <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17" style="4" customWidth="1"/>
-    <col min="3" max="3" width="20.125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="20.375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="26.625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="22.5" style="4" customWidth="1"/>
-    <col min="7" max="7" width="23.875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20.375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="18.375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="59.5" style="4" customWidth="1"/>
-    <col min="11" max="11" width="18.875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="13.5" style="4" customWidth="1"/>
-    <col min="13" max="13" width="20" style="4" customWidth="1"/>
-    <col min="14" max="14" width="30.125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="24.25" style="4" customWidth="1"/>
-    <col min="16" max="26" width="9.375" style="4" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="4"/>
+    <col min="1" max="1" width="18.375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="17" style="6" customWidth="1"/>
+    <col min="3" max="3" width="20.125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="42.75" style="6" customWidth="1"/>
+    <col min="5" max="5" width="48.625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="22.5" style="6" customWidth="1"/>
+    <col min="7" max="7" width="23.875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="20.375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="18.375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="59.5" style="6" customWidth="1"/>
+    <col min="11" max="11" width="18.875" style="6" customWidth="1"/>
+    <col min="12" max="12" width="13.5" style="6" customWidth="1"/>
+    <col min="13" max="13" width="20" style="6" customWidth="1"/>
+    <col min="14" max="14" width="30.125" style="6" customWidth="1"/>
+    <col min="15" max="15" width="24.25" style="6" customWidth="1"/>
+    <col min="16" max="26" width="9.375" style="6" customWidth="1"/>
+    <col min="27" max="16384" width="12.625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="7" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="9">
-        <v>593987648370</v>
-      </c>
-      <c r="E2" s="9">
-        <v>2.02008231047449E+16</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="8">
-        <v>2</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="8">
-        <v>1734</v>
-      </c>
-      <c r="L2" s="8">
-        <v>1</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="8">
-        <v>3</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="9">
-        <v>593987648370</v>
-      </c>
-      <c r="E3" s="9">
-        <v>2.02008231047449E+16</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="8">
-        <v>1</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="8">
-        <v>1821</v>
-      </c>
-      <c r="L3" s="8">
-        <v>1</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="8">
-        <v>3</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="5">
-        <v>593999851126</v>
-      </c>
-      <c r="E4" s="5">
-        <v>2.02008231305171E+16</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="3">
-        <v>1</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="3">
-        <v>1808</v>
-      </c>
-      <c r="L4" s="3">
-        <v>1</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" s="3">
-        <v>1</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1" spans="1:15" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+    </row>
+    <row r="2" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4787,6 +3885,6 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>